<commit_message>
Upgraded API to v2.5.0
</commit_message>
<xml_diff>
--- a/documents/Published/Bowtie Chart/BowtieByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Bowtie Chart/BowtieByMAQSoftwareChecklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18518"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\Desktop\Bowtie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual\documents\Published\Bowtie Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCB1B19-E231-4D23-90F6-4263B3D503B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{57A5B581-B042-464E-A8EB-9743E2CFC5B3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{57A5B581-B042-464E-A8EB-9743E2CFC5B3}"/>
   </bookViews>
   <sheets>
     <sheet name="BVT" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>S no</t>
   </si>
@@ -282,6 +283,21 @@
   </si>
   <si>
     <t>Does visual legends adjusted on resizing? </t>
+  </si>
+  <si>
+    <t>PowerBi</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>Internet Exp</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -414,24 +430,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -450,6 +448,24 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,6 +481,891 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>202406</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2365487</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1428750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F71C54AC-A0F6-4D78-BFE4-30FC5EC9FB75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10322719" y="285750"/>
+          <a:ext cx="2163081" cy="1333500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>154782</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>59532</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2398089</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1464470</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A53DA1E-D4B9-4229-902B-4E92533A6803}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10275095" y="2214563"/>
+          <a:ext cx="2243307" cy="1404938"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>511968</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>83345</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2312611</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1559719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28E06CFA-0DA6-4865-99E6-92BEF435E67A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10632281" y="3940970"/>
+          <a:ext cx="1800643" cy="1476374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>297655</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>50461</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2421461</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1559719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E24047CA-7EC0-4180-ABCB-75B91205427F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10417968" y="5574961"/>
+          <a:ext cx="2123806" cy="1509258"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>142873</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2536030</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1684066</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38F5EECE-8425-4EAE-8607-AE1E7C04572B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10263186" y="7465219"/>
+          <a:ext cx="2393157" cy="1517378"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>154782</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>83344</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2560646</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1690688</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAA2375F-CD4E-4B8C-8DBB-C8A4FE91ED66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12894470" y="273844"/>
+          <a:ext cx="2405864" cy="1607344"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>345282</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>130969</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2452688</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1528417</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFAA3F6D-F236-4C3F-8104-E24E1283E5DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13084970" y="2286000"/>
+          <a:ext cx="2107406" cy="1397448"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>37449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2524124</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1519116</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77FB4FF5-808C-48FE-99E8-36A9DC8B7255}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13096875" y="3895074"/>
+          <a:ext cx="2166937" cy="1481667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>226218</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>64717</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2591407</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1586304</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F72D8690-67D3-4DCD-BDBD-FCEDA86A523B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12965906" y="5589217"/>
+          <a:ext cx="2365189" cy="1521587"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>71436</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>265043</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2627405</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1364838</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95CEDEE2-EBE3-4FEC-88DB-36B32FA8D90C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12811124" y="7563574"/>
+          <a:ext cx="2555969" cy="1099795"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>202406</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2928083</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1559719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9F8C154-79CE-4A4D-B631-DFFA0BE2DA21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15525751" y="7500937"/>
+          <a:ext cx="2785207" cy="1357313"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>321469</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>176865</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3167741</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1538611</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12BE489B-D21C-485D-8A51-F54C6D192CE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15704344" y="5701365"/>
+          <a:ext cx="2846272" cy="1361746"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>189291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2996294</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1331446</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28BB78B5-7EBC-4A74-AF2C-E6B3A67F0C9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16002000" y="4046916"/>
+          <a:ext cx="2377169" cy="1142155"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>440532</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3000376</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1712406</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93F3A522-1CB3-489D-8A04-556BB8C83694}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15823407" y="333375"/>
+          <a:ext cx="2559844" cy="1569531"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>154781</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>226219</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>3025924</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1416844</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{010833D2-E174-4401-BD11-5719F56D0295}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15537656" y="2381250"/>
+          <a:ext cx="2871143" cy="1190625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2945536</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1837472</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B83651F1-DEB9-4F33-B1C8-87B2EEE402B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18764251" y="309562"/>
+          <a:ext cx="2802660" cy="1718410"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>11906</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>226218</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2963785</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1357312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{565314B9-1C44-4522-9F18-41F1BAB8BCC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18633281" y="2559843"/>
+          <a:ext cx="2951879" cy="1131094"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>178594</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2803206</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1357312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{382753B8-6884-4EED-8878-21B2F766DA9E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18669000" y="4214813"/>
+          <a:ext cx="2755581" cy="1178718"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>122167</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>214312</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2855844</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1309688</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAD5B3AC-7A32-41AA-9538-3BF407243556}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18743542" y="5917406"/>
+          <a:ext cx="2733677" cy="1095376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>56362</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>107156</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1552885</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91C11DD2-0490-4480-864F-139458B953A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18677737" y="7584281"/>
+          <a:ext cx="2801138" cy="1445729"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -764,10 +1665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE24082D-17DB-42D9-AF44-9F2CC3ACE4ED}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,9 +1677,13 @@
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
     <col min="4" max="4" width="37.7109375" customWidth="1"/>
     <col min="5" max="5" width="40.28515625" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" customWidth="1"/>
+    <col min="8" max="8" width="48.5703125" customWidth="1"/>
+    <col min="9" max="9" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -794,8 +1699,20 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -811,8 +1728,20 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -828,8 +1757,20 @@
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -845,8 +1786,20 @@
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -862,8 +1815,20 @@
       <c r="E5" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -878,11 +1843,24 @@
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1076,29 +2054,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="13">
         <v>16</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="17"/>
     </row>
     <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="18" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="18"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
@@ -1112,41 +2090,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="13">
         <v>18</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="14"/>
+      <c r="B22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="17"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="14"/>
+      <c r="B23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="17"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="17"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="15" t="s">
+      <c r="A25" s="15"/>
+      <c r="B25" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="18"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5">

</xml_diff>